<commit_message>
Let's add more dummy demo projects
</commit_message>
<xml_diff>
--- a/db/demo.xlsx
+++ b/db/demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Resource Allocation Worksheet" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="42">
   <si>
     <t>Status</t>
   </si>
@@ -75,15 +75,78 @@
   <si>
     <t>William Kinard</t>
   </si>
+  <si>
+    <t>The Spitzer Foundation</t>
+  </si>
+  <si>
+    <t>SOW1 - Telescope MVP</t>
+  </si>
+  <si>
+    <t>Recurring</t>
+  </si>
+  <si>
+    <t>Intridea</t>
+  </si>
+  <si>
+    <t>Internal::Paid Time Off</t>
+  </si>
+  <si>
+    <t>Voyager</t>
+  </si>
+  <si>
+    <t>SOW1 - Interstellar Space</t>
+  </si>
+  <si>
+    <t>SOW2 - Heliosheath</t>
+  </si>
+  <si>
+    <t>Spirit &amp; Opportunity</t>
+  </si>
+  <si>
+    <t>SOW1 - Mars</t>
+  </si>
+  <si>
+    <t>Cassini-Huygens</t>
+  </si>
+  <si>
+    <t>SOW1 - Saturn</t>
+  </si>
+  <si>
+    <t>SOW2 - Moon</t>
+  </si>
+  <si>
+    <t>Chandra</t>
+  </si>
+  <si>
+    <t>SOW1 - Cassiopeia A</t>
+  </si>
+  <si>
+    <t>Viking 1</t>
+  </si>
+  <si>
+    <t>Hubble</t>
+  </si>
+  <si>
+    <t>SOW1 - Space Telescope</t>
+  </si>
+  <si>
+    <t>Apollo </t>
+  </si>
+  <si>
+    <t>SOW13 - Moon</t>
+  </si>
+  <si>
+    <t>Apollo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="m/d;@"/>
-    <numFmt numFmtId="166" formatCode="m/d;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -123,15 +186,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="6.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <strike val="0"/>
@@ -146,6 +200,15 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="6.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -209,20 +272,20 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="0" applyFont="1" fontId="3" applyNumberFormat="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="165" borderId="0" applyFont="1" fontId="5" applyNumberFormat="1" applyFill="1">
+    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="164" borderId="0" applyFont="1" fontId="4" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center" horizontal="right" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="165" borderId="0" applyFont="1" fontId="5" applyNumberFormat="1">
+      <alignment vertical="center" horizontal="general" wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="166" borderId="0" applyFont="1" fontId="6" applyNumberFormat="1">
-      <alignment vertical="center" horizontal="general" wrapText="1"/>
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="7">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
@@ -231,7 +294,37 @@
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF6AA84F"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB6D7A8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF999999"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFBF9000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF6AA84F"/>
@@ -262,26 +355,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF6AA84F"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFB6D7A8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF999999"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFD9D9D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
 </styleSheet>
 </file>
@@ -290,412 +363,414 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane topLeftCell="A3" ySplit="2.0" activePane="bottomLeft" state="frozen"/>
+      <pane topLeftCell="G3" ySplit="2.0" xSplit="6.0" activePane="bottomRight" state="frozen"/>
+      <selection sqref="G1" activeCell="G1" pane="topRight"/>
       <selection sqref="A3" activeCell="A3" pane="bottomLeft"/>
+      <selection sqref="G3" activeCell="G3" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="14.29"/>
-    <col min="2" customWidth="1" max="2" width="4.86"/>
+    <col min="1" customWidth="1" max="1" width="5.71"/>
+    <col min="2" customWidth="1" max="2" width="1.43"/>
     <col min="4" customWidth="1" max="4" width="23.71"/>
-    <col min="5" customWidth="1" max="5" width="27.71"/>
+    <col min="5" customWidth="1" max="5" width="25.86"/>
     <col min="6" customWidth="1" max="6" width="6.57"/>
-    <col min="7" customWidth="1" max="7" width="5.86"/>
+    <col min="7" customWidth="1" max="7" width="4.71"/>
     <col min="8" customWidth="1" max="60" width="6.0"/>
   </cols>
   <sheetData>
     <row customHeight="1" r="1" ht="19.5">
-      <c t="s" s="7" r="A1">
+      <c t="s" s="6" r="A1">
         <v>0</v>
       </c>
-      <c s="7" r="B1"/>
-      <c t="s" s="7" r="C1">
+      <c s="6" r="B1"/>
+      <c t="s" s="6" r="C1">
         <v>1</v>
       </c>
-      <c t="s" s="7" r="D1">
+      <c t="s" s="6" r="D1">
         <v>2</v>
       </c>
-      <c t="s" s="7" r="E1">
+      <c t="s" s="6" r="E1">
         <v>3</v>
       </c>
-      <c t="s" s="7" r="F1">
+      <c t="s" s="6" r="F1">
         <v>4</v>
       </c>
-      <c t="s" s="5" r="G1">
+      <c t="s" s="4" r="G1">
         <v>5</v>
       </c>
-      <c s="7" r="H1">
+      <c s="6" r="H1">
         <v>41644</v>
       </c>
-      <c s="7" r="I1">
+      <c s="6" r="I1">
         <v>41651</v>
       </c>
-      <c s="7" r="J1">
+      <c s="6" r="J1">
         <v>41658</v>
       </c>
-      <c s="7" r="K1">
+      <c s="6" r="K1">
         <v>41665</v>
       </c>
-      <c s="7" r="L1">
+      <c s="6" r="L1">
         <v>41672</v>
       </c>
-      <c s="7" r="M1">
+      <c s="6" r="M1">
         <v>41679</v>
       </c>
-      <c s="7" r="N1">
+      <c s="6" r="N1">
         <v>41686</v>
       </c>
-      <c s="7" r="O1">
+      <c s="6" r="O1">
         <v>41693</v>
       </c>
-      <c s="7" r="P1">
+      <c s="6" r="P1">
         <v>41700</v>
       </c>
-      <c s="7" r="Q1">
+      <c s="6" r="Q1">
         <v>41707</v>
       </c>
-      <c s="7" r="R1">
+      <c s="6" r="R1">
         <v>41714</v>
       </c>
-      <c s="7" r="S1">
+      <c s="6" r="S1">
         <v>41721</v>
       </c>
-      <c s="7" r="T1">
+      <c s="6" r="T1">
         <v>41728</v>
       </c>
-      <c s="7" r="U1">
+      <c s="6" r="U1">
         <v>41735</v>
       </c>
-      <c s="7" r="V1">
+      <c s="6" r="V1">
         <v>41742</v>
       </c>
-      <c s="7" r="W1">
+      <c s="6" r="W1">
         <v>41749</v>
       </c>
-      <c s="7" r="X1">
+      <c s="6" r="X1">
         <v>41756</v>
       </c>
-      <c s="7" r="Y1">
+      <c s="6" r="Y1">
         <v>41763</v>
       </c>
-      <c s="7" r="Z1">
+      <c s="6" r="Z1">
         <v>41770</v>
       </c>
-      <c s="7" r="AA1">
+      <c s="6" r="AA1">
         <v>41777</v>
       </c>
-      <c s="7" r="AB1">
+      <c s="6" r="AB1">
         <v>41784</v>
       </c>
-      <c s="7" r="AC1">
+      <c s="6" r="AC1">
         <v>41791</v>
       </c>
-      <c s="7" r="AD1">
+      <c s="6" r="AD1">
         <v>41798</v>
       </c>
-      <c s="7" r="AE1">
+      <c s="6" r="AE1">
         <v>41805</v>
       </c>
-      <c s="7" r="AF1">
+      <c s="6" r="AF1">
         <v>41812</v>
       </c>
-      <c s="7" r="AG1">
+      <c s="6" r="AG1">
         <v>41819</v>
       </c>
-      <c s="7" r="AH1">
+      <c s="6" r="AH1">
         <v>41826</v>
       </c>
-      <c s="7" r="AI1">
+      <c s="6" r="AI1">
         <v>41833</v>
       </c>
-      <c s="7" r="AJ1">
+      <c s="6" r="AJ1">
         <v>41840</v>
       </c>
-      <c s="7" r="AK1">
+      <c s="6" r="AK1">
         <v>41847</v>
       </c>
-      <c s="7" r="AL1">
+      <c s="6" r="AL1">
         <v>41854</v>
       </c>
-      <c s="7" r="AM1">
+      <c s="6" r="AM1">
         <v>41861</v>
       </c>
-      <c s="7" r="AN1">
+      <c s="6" r="AN1">
         <v>41868</v>
       </c>
-      <c s="7" r="AO1">
+      <c s="6" r="AO1">
         <v>41875</v>
       </c>
-      <c s="7" r="AP1">
+      <c s="6" r="AP1">
         <v>41882</v>
       </c>
-      <c s="7" r="AQ1">
+      <c s="6" r="AQ1">
         <v>41889</v>
       </c>
-      <c s="7" r="AR1">
+      <c s="6" r="AR1">
         <v>41896</v>
       </c>
-      <c s="7" r="AS1">
+      <c s="6" r="AS1">
         <v>41903</v>
       </c>
-      <c s="7" r="AT1">
+      <c s="6" r="AT1">
         <v>41910</v>
       </c>
-      <c s="7" r="AU1">
+      <c s="6" r="AU1">
         <v>41917</v>
       </c>
-      <c s="7" r="AV1">
+      <c s="6" r="AV1">
         <v>41924</v>
       </c>
-      <c s="7" r="AW1">
+      <c s="6" r="AW1">
         <v>41931</v>
       </c>
-      <c s="7" r="AX1">
+      <c s="6" r="AX1">
         <v>41938</v>
       </c>
-      <c s="7" r="AY1">
+      <c s="6" r="AY1">
         <v>41945</v>
       </c>
-      <c s="7" r="AZ1">
+      <c s="6" r="AZ1">
         <v>41952</v>
       </c>
-      <c s="7" r="BA1">
+      <c s="6" r="BA1">
         <v>41959</v>
       </c>
-      <c s="7" r="BB1">
+      <c s="6" r="BB1">
         <v>41966</v>
       </c>
-      <c s="7" r="BC1">
+      <c s="6" r="BC1">
         <v>41973</v>
       </c>
-      <c s="7" r="BD1">
+      <c s="6" r="BD1">
         <v>41980</v>
       </c>
-      <c s="7" r="BE1">
+      <c s="6" r="BE1">
         <v>41987</v>
       </c>
-      <c s="7" r="BF1">
+      <c s="6" r="BF1">
         <v>41994</v>
       </c>
-      <c s="7" r="BG1">
+      <c s="6" r="BG1">
         <v>42001</v>
       </c>
-      <c s="7" r="BH1"/>
+      <c s="6" r="BH1"/>
     </row>
     <row customHeight="1" r="2" ht="1.5">
       <c s="2" r="A2"/>
-      <c s="4" r="B2"/>
+      <c s="3" r="B2"/>
       <c s="8" r="C2"/>
       <c s="8" r="D2"/>
       <c s="8" r="E2"/>
       <c s="8" r="F2"/>
       <c s="1" r="G2"/>
-      <c s="3" r="H2">
+      <c s="7" r="H2">
         <f>H1</f>
         <v>41644</v>
       </c>
-      <c s="3" r="I2">
+      <c s="7" r="I2">
         <f>H1</f>
         <v>41644</v>
       </c>
-      <c s="3" r="J2">
+      <c s="7" r="J2">
         <f>I1</f>
         <v>41651</v>
       </c>
-      <c s="3" r="K2">
+      <c s="7" r="K2">
         <f>J1</f>
         <v>41658</v>
       </c>
-      <c s="3" r="L2">
+      <c s="7" r="L2">
         <f>K1</f>
         <v>41665</v>
       </c>
-      <c s="3" r="M2">
+      <c s="7" r="M2">
         <f>L1</f>
         <v>41672</v>
       </c>
-      <c s="3" r="N2">
+      <c s="7" r="N2">
         <f>M1</f>
         <v>41679</v>
       </c>
-      <c s="3" r="O2">
+      <c s="7" r="O2">
         <f>N1</f>
         <v>41686</v>
       </c>
-      <c s="3" r="P2">
+      <c s="7" r="P2">
         <f>O1</f>
         <v>41693</v>
       </c>
-      <c s="3" r="Q2">
+      <c s="7" r="Q2">
         <f>P1</f>
         <v>41700</v>
       </c>
-      <c s="3" r="R2">
+      <c s="7" r="R2">
         <f>Q1</f>
         <v>41707</v>
       </c>
-      <c s="3" r="S2">
+      <c s="7" r="S2">
         <f>R1</f>
         <v>41714</v>
       </c>
-      <c s="3" r="T2">
+      <c s="7" r="T2">
         <f>S1</f>
         <v>41721</v>
       </c>
-      <c s="3" r="U2">
+      <c s="7" r="U2">
         <f>T1</f>
         <v>41728</v>
       </c>
-      <c s="3" r="V2">
+      <c s="7" r="V2">
         <f>U1</f>
         <v>41735</v>
       </c>
-      <c s="3" r="W2">
+      <c s="7" r="W2">
         <f>V1</f>
         <v>41742</v>
       </c>
-      <c s="3" r="X2">
+      <c s="7" r="X2">
         <f>W1</f>
         <v>41749</v>
       </c>
-      <c s="3" r="Y2">
+      <c s="7" r="Y2">
         <f>X1</f>
         <v>41756</v>
       </c>
-      <c s="3" r="Z2">
+      <c s="7" r="Z2">
         <f>Y1</f>
         <v>41763</v>
       </c>
-      <c s="3" r="AA2">
+      <c s="7" r="AA2">
         <f>Z1</f>
         <v>41770</v>
       </c>
-      <c s="3" r="AB2">
+      <c s="7" r="AB2">
         <f>AA1</f>
         <v>41777</v>
       </c>
-      <c s="3" r="AC2">
+      <c s="7" r="AC2">
         <f>AB1</f>
         <v>41784</v>
       </c>
-      <c s="3" r="AD2">
+      <c s="7" r="AD2">
         <f>AC1</f>
         <v>41791</v>
       </c>
-      <c s="3" r="AE2">
+      <c s="7" r="AE2">
         <f>AD1</f>
         <v>41798</v>
       </c>
-      <c s="3" r="AF2">
+      <c s="7" r="AF2">
         <f>AE1</f>
         <v>41805</v>
       </c>
-      <c s="3" r="AG2">
+      <c s="7" r="AG2">
         <f>AF1</f>
         <v>41812</v>
       </c>
-      <c s="3" r="AH2">
+      <c s="7" r="AH2">
         <f>AG1</f>
         <v>41819</v>
       </c>
-      <c s="3" r="AI2">
+      <c s="7" r="AI2">
         <f>AH1</f>
         <v>41826</v>
       </c>
-      <c s="3" r="AJ2">
+      <c s="7" r="AJ2">
         <f>AI1</f>
         <v>41833</v>
       </c>
-      <c s="3" r="AK2">
+      <c s="7" r="AK2">
         <f>AJ1</f>
         <v>41840</v>
       </c>
-      <c s="3" r="AL2">
+      <c s="7" r="AL2">
         <f>AK1</f>
         <v>41847</v>
       </c>
-      <c s="3" r="AM2">
+      <c s="7" r="AM2">
         <f>AL1</f>
         <v>41854</v>
       </c>
-      <c s="3" r="AN2">
+      <c s="7" r="AN2">
         <f>AM1</f>
         <v>41861</v>
       </c>
-      <c s="3" r="AO2">
+      <c s="7" r="AO2">
         <f>AN1</f>
         <v>41868</v>
       </c>
-      <c s="3" r="AP2">
+      <c s="7" r="AP2">
         <f>AO1</f>
         <v>41875</v>
       </c>
-      <c s="3" r="AQ2">
+      <c s="7" r="AQ2">
         <f>AP1</f>
         <v>41882</v>
       </c>
-      <c s="3" r="AR2">
+      <c s="7" r="AR2">
         <f>AQ1</f>
         <v>41889</v>
       </c>
-      <c s="3" r="AS2">
+      <c s="7" r="AS2">
         <f>AR1</f>
         <v>41896</v>
       </c>
-      <c s="3" r="AT2">
+      <c s="7" r="AT2">
         <f>AS1</f>
         <v>41903</v>
       </c>
-      <c s="3" r="AU2">
+      <c s="7" r="AU2">
         <f>AT1</f>
         <v>41910</v>
       </c>
-      <c s="3" r="AV2">
+      <c s="7" r="AV2">
         <f>AU1</f>
         <v>41917</v>
       </c>
-      <c s="3" r="AW2">
+      <c s="7" r="AW2">
         <f>AV1</f>
         <v>41924</v>
       </c>
-      <c s="3" r="AX2">
+      <c s="7" r="AX2">
         <f>AW1</f>
         <v>41931</v>
       </c>
-      <c s="3" r="AY2">
+      <c s="7" r="AY2">
         <f>AX1</f>
         <v>41938</v>
       </c>
-      <c s="3" r="AZ2">
+      <c s="7" r="AZ2">
         <f>AY1</f>
         <v>41945</v>
       </c>
-      <c s="3" r="BA2">
+      <c s="7" r="BA2">
         <f>AZ1</f>
         <v>41952</v>
       </c>
-      <c s="3" r="BB2">
+      <c s="7" r="BB2">
         <f>BA1</f>
         <v>41959</v>
       </c>
-      <c s="3" r="BC2">
+      <c s="7" r="BC2">
         <f>BB1</f>
         <v>41966</v>
       </c>
-      <c s="3" r="BD2">
+      <c s="7" r="BD2">
         <f>BC1</f>
         <v>41973</v>
       </c>
-      <c s="3" r="BE2">
+      <c s="7" r="BE2">
         <f>BD1</f>
         <v>41980</v>
       </c>
-      <c s="3" r="BF2">
+      <c s="7" r="BF2">
         <f>BE1</f>
         <v>41987</v>
       </c>
-      <c s="3" r="BG2">
+      <c s="7" r="BG2">
         <f>BF1</f>
         <v>41994</v>
       </c>
@@ -717,13 +792,7 @@
       <c t="s" r="F3">
         <v>10</v>
       </c>
-      <c s="6" r="G3"/>
-      <c r="N3">
-        <v>20</v>
-      </c>
-      <c r="O3">
-        <v>30</v>
-      </c>
+      <c s="5" r="G3"/>
       <c r="P3">
         <v>40</v>
       </c>
@@ -792,13 +861,7 @@
       <c t="s" r="F4">
         <v>10</v>
       </c>
-      <c s="6" r="G4"/>
-      <c r="N4">
-        <v>20</v>
-      </c>
-      <c r="O4">
-        <v>30</v>
-      </c>
+      <c s="5" r="G4"/>
       <c r="P4">
         <v>40</v>
       </c>
@@ -867,13 +930,7 @@
       <c t="s" r="F5">
         <v>14</v>
       </c>
-      <c s="6" r="G5"/>
-      <c r="N5">
-        <v>40</v>
-      </c>
-      <c r="O5">
-        <v>20</v>
-      </c>
+      <c s="5" r="G5"/>
       <c r="P5">
         <v>20</v>
       </c>
@@ -942,13 +999,7 @@
       <c t="s" r="F6">
         <v>16</v>
       </c>
-      <c s="6" r="G6"/>
-      <c r="N6">
-        <v>36</v>
-      </c>
-      <c r="O6">
-        <v>18</v>
-      </c>
+      <c s="5" r="G6"/>
       <c r="P6">
         <v>24</v>
       </c>
@@ -1017,13 +1068,7 @@
       <c t="s" r="F7">
         <v>16</v>
       </c>
-      <c s="6" r="G7"/>
-      <c r="N7">
-        <v>8</v>
-      </c>
-      <c r="O7">
-        <v>16</v>
-      </c>
+      <c s="5" r="G7"/>
       <c r="P7">
         <v>16</v>
       </c>
@@ -1092,7 +1137,7 @@
       <c t="s" r="F8">
         <v>14</v>
       </c>
-      <c s="6" r="G8"/>
+      <c s="5" r="G8"/>
       <c r="R8">
         <v>20</v>
       </c>
@@ -1179,7 +1224,7 @@
       <c t="s" r="F9">
         <v>16</v>
       </c>
-      <c s="6" r="G9"/>
+      <c s="5" r="G9"/>
       <c r="R9">
         <v>16</v>
       </c>
@@ -1266,7 +1311,7 @@
       <c t="s" r="F10">
         <v>16</v>
       </c>
-      <c s="6" r="G10"/>
+      <c s="5" r="G10"/>
       <c r="R10">
         <v>24</v>
       </c>
@@ -1353,7 +1398,7 @@
       <c t="s" r="F11">
         <v>10</v>
       </c>
-      <c s="6" r="G11"/>
+      <c s="5" r="G11"/>
       <c r="R11">
         <v>40</v>
       </c>
@@ -1440,7 +1485,7 @@
       <c t="s" r="F12">
         <v>10</v>
       </c>
-      <c s="6" r="G12"/>
+      <c s="5" r="G12"/>
       <c r="R12">
         <v>40</v>
       </c>
@@ -1512,280 +1557,3167 @@
       </c>
     </row>
     <row customHeight="1" r="13" ht="19.5">
-      <c s="6" r="G13"/>
+      <c t="s" r="A13">
+        <v>6</v>
+      </c>
+      <c t="s" r="C13">
+        <v>13</v>
+      </c>
+      <c t="s" r="D13">
+        <v>21</v>
+      </c>
+      <c t="s" r="E13">
+        <v>22</v>
+      </c>
+      <c t="s" r="F13">
+        <v>14</v>
+      </c>
+      <c s="5" r="G13"/>
+      <c r="J13">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <v>20</v>
+      </c>
+      <c r="L13">
+        <v>20</v>
+      </c>
+      <c r="M13">
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <v>20</v>
+      </c>
+      <c r="O13">
+        <v>20</v>
+      </c>
+      <c r="P13">
+        <v>20</v>
+      </c>
     </row>
     <row customHeight="1" r="14" ht="19.5">
-      <c s="6" r="G14"/>
+      <c t="s" r="A14">
+        <v>6</v>
+      </c>
+      <c t="s" r="C14">
+        <v>15</v>
+      </c>
+      <c t="s" r="D14">
+        <v>21</v>
+      </c>
+      <c t="s" r="E14">
+        <v>22</v>
+      </c>
+      <c t="s" r="F14">
+        <v>16</v>
+      </c>
+      <c s="5" r="G14"/>
+      <c r="J14">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>16</v>
+      </c>
+      <c r="L14">
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <v>16</v>
+      </c>
+      <c r="N14">
+        <v>16</v>
+      </c>
+      <c r="O14">
+        <v>16</v>
+      </c>
+      <c r="P14">
+        <v>16</v>
+      </c>
     </row>
     <row customHeight="1" r="15" ht="19.5">
-      <c s="6" r="G15"/>
+      <c t="s" r="A15">
+        <v>6</v>
+      </c>
+      <c t="s" r="C15">
+        <v>17</v>
+      </c>
+      <c t="s" r="D15">
+        <v>21</v>
+      </c>
+      <c t="s" r="E15">
+        <v>22</v>
+      </c>
+      <c t="s" r="F15">
+        <v>16</v>
+      </c>
+      <c s="5" r="G15"/>
+      <c r="J15">
+        <v>24</v>
+      </c>
+      <c r="K15">
+        <v>24</v>
+      </c>
+      <c r="L15">
+        <v>24</v>
+      </c>
+      <c r="M15">
+        <v>24</v>
+      </c>
+      <c r="N15">
+        <v>24</v>
+      </c>
+      <c r="O15">
+        <v>24</v>
+      </c>
+      <c r="P15">
+        <v>24</v>
+      </c>
     </row>
     <row customHeight="1" r="16" ht="19.5">
-      <c s="6" r="G16"/>
+      <c t="s" r="A16">
+        <v>6</v>
+      </c>
+      <c t="s" r="C16">
+        <v>19</v>
+      </c>
+      <c t="s" r="D16">
+        <v>21</v>
+      </c>
+      <c t="s" r="E16">
+        <v>22</v>
+      </c>
+      <c t="s" r="F16">
+        <v>10</v>
+      </c>
+      <c s="5" r="G16"/>
+      <c r="J16">
+        <v>40</v>
+      </c>
+      <c r="K16">
+        <v>40</v>
+      </c>
+      <c r="L16">
+        <v>40</v>
+      </c>
+      <c r="M16">
+        <v>40</v>
+      </c>
+      <c r="N16">
+        <v>40</v>
+      </c>
+      <c r="O16">
+        <v>40</v>
+      </c>
+      <c r="P16">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="17" ht="19.5">
-      <c s="6" r="G17"/>
+      <c t="s" r="A17">
+        <v>6</v>
+      </c>
+      <c t="s" r="C17">
+        <v>20</v>
+      </c>
+      <c t="s" r="D17">
+        <v>21</v>
+      </c>
+      <c t="s" r="E17">
+        <v>22</v>
+      </c>
+      <c t="s" r="F17">
+        <v>10</v>
+      </c>
+      <c s="5" r="G17"/>
+      <c r="J17">
+        <v>40</v>
+      </c>
+      <c r="K17">
+        <v>40</v>
+      </c>
+      <c r="L17">
+        <v>40</v>
+      </c>
+      <c r="M17">
+        <v>40</v>
+      </c>
+      <c r="N17">
+        <v>40</v>
+      </c>
+      <c r="O17">
+        <v>40</v>
+      </c>
+      <c r="P17">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="18" ht="19.5">
-      <c s="6" r="G18"/>
+      <c t="s" r="A18">
+        <v>23</v>
+      </c>
+      <c t="s" r="C18">
+        <v>17</v>
+      </c>
+      <c t="s" r="D18">
+        <v>24</v>
+      </c>
+      <c t="s" r="E18">
+        <v>25</v>
+      </c>
+      <c t="s" r="F18">
+        <v>16</v>
+      </c>
+      <c s="5" r="G18"/>
+      <c r="Q18">
+        <f>3*8</f>
+        <v>24</v>
+      </c>
     </row>
     <row customHeight="1" r="19" ht="19.5">
-      <c s="6" r="G19"/>
+      <c t="s" r="A19">
+        <v>6</v>
+      </c>
+      <c t="s" r="C19">
+        <v>13</v>
+      </c>
+      <c t="s" r="D19">
+        <v>26</v>
+      </c>
+      <c t="s" r="E19">
+        <v>27</v>
+      </c>
+      <c t="s" r="F19">
+        <v>14</v>
+      </c>
+      <c s="5" r="G19"/>
+      <c r="AL19">
+        <v>40</v>
+      </c>
+      <c r="AM19">
+        <v>40</v>
+      </c>
+      <c r="AN19">
+        <v>40</v>
+      </c>
+      <c r="AO19">
+        <v>40</v>
+      </c>
+      <c r="AP19">
+        <v>20</v>
+      </c>
+      <c r="AQ19">
+        <v>20</v>
+      </c>
     </row>
     <row customHeight="1" r="20" ht="19.5">
-      <c s="6" r="G20"/>
+      <c t="s" r="A20">
+        <v>6</v>
+      </c>
+      <c t="s" r="C20">
+        <v>15</v>
+      </c>
+      <c t="s" r="D20">
+        <v>26</v>
+      </c>
+      <c t="s" r="E20">
+        <v>27</v>
+      </c>
+      <c t="s" r="F20">
+        <v>16</v>
+      </c>
+      <c s="5" r="G20"/>
+      <c r="AL20">
+        <v>40</v>
+      </c>
+      <c r="AM20">
+        <v>40</v>
+      </c>
+      <c r="AN20">
+        <v>40</v>
+      </c>
+      <c r="AO20">
+        <v>40</v>
+      </c>
+      <c r="AP20">
+        <v>20</v>
+      </c>
+      <c r="AQ20">
+        <v>20</v>
+      </c>
     </row>
     <row customHeight="1" r="21" ht="19.5">
-      <c s="6" r="G21"/>
+      <c t="s" r="A21">
+        <v>6</v>
+      </c>
+      <c t="s" r="C21">
+        <v>17</v>
+      </c>
+      <c t="s" r="D21">
+        <v>26</v>
+      </c>
+      <c t="s" r="E21">
+        <v>27</v>
+      </c>
+      <c t="s" r="F21">
+        <v>16</v>
+      </c>
+      <c s="5" r="G21"/>
+      <c r="AL21">
+        <v>40</v>
+      </c>
+      <c r="AM21">
+        <v>40</v>
+      </c>
+      <c r="AN21">
+        <v>40</v>
+      </c>
+      <c r="AO21">
+        <v>40</v>
+      </c>
+      <c r="AP21">
+        <v>20</v>
+      </c>
+      <c r="AQ21">
+        <v>20</v>
+      </c>
     </row>
     <row customHeight="1" r="22" ht="19.5">
-      <c s="6" r="G22"/>
+      <c t="s" r="A22">
+        <v>6</v>
+      </c>
+      <c t="s" r="C22">
+        <v>19</v>
+      </c>
+      <c t="s" r="D22">
+        <v>26</v>
+      </c>
+      <c t="s" r="E22">
+        <v>27</v>
+      </c>
+      <c t="s" r="F22">
+        <v>10</v>
+      </c>
+      <c s="5" r="G22"/>
+      <c r="AL22">
+        <v>40</v>
+      </c>
+      <c r="AM22">
+        <v>40</v>
+      </c>
+      <c r="AN22">
+        <v>40</v>
+      </c>
+      <c r="AO22">
+        <v>40</v>
+      </c>
+      <c r="AP22">
+        <v>20</v>
+      </c>
+      <c r="AQ22">
+        <v>20</v>
+      </c>
     </row>
     <row customHeight="1" r="23" ht="19.5">
-      <c s="6" r="G23"/>
+      <c t="s" r="A23">
+        <v>6</v>
+      </c>
+      <c t="s" r="C23">
+        <v>20</v>
+      </c>
+      <c t="s" r="D23">
+        <v>26</v>
+      </c>
+      <c t="s" r="E23">
+        <v>27</v>
+      </c>
+      <c t="s" r="F23">
+        <v>10</v>
+      </c>
+      <c s="5" r="G23"/>
+      <c r="AL23">
+        <v>40</v>
+      </c>
+      <c r="AM23">
+        <v>40</v>
+      </c>
+      <c r="AN23">
+        <v>40</v>
+      </c>
+      <c r="AO23">
+        <v>40</v>
+      </c>
+      <c r="AP23">
+        <v>20</v>
+      </c>
+      <c r="AQ23">
+        <v>20</v>
+      </c>
     </row>
     <row customHeight="1" r="24" ht="19.5">
-      <c s="6" r="G24"/>
+      <c t="s" r="A24">
+        <v>6</v>
+      </c>
+      <c t="s" r="C24">
+        <v>13</v>
+      </c>
+      <c t="s" r="D24">
+        <v>26</v>
+      </c>
+      <c t="s" r="E24">
+        <v>28</v>
+      </c>
+      <c t="s" r="F24">
+        <v>14</v>
+      </c>
+      <c s="5" r="G24"/>
+      <c r="AP24">
+        <v>20</v>
+      </c>
+      <c r="AQ24">
+        <v>20</v>
+      </c>
+      <c r="AR24">
+        <v>40</v>
+      </c>
+      <c r="AS24">
+        <v>40</v>
+      </c>
+      <c r="AT24">
+        <v>40</v>
+      </c>
+      <c r="AU24">
+        <v>40</v>
+      </c>
+      <c r="AV24">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="25" ht="19.5">
-      <c s="6" r="G25"/>
+      <c t="s" r="A25">
+        <v>6</v>
+      </c>
+      <c t="s" r="C25">
+        <v>15</v>
+      </c>
+      <c t="s" r="D25">
+        <v>26</v>
+      </c>
+      <c t="s" r="E25">
+        <v>28</v>
+      </c>
+      <c t="s" r="F25">
+        <v>16</v>
+      </c>
+      <c s="5" r="G25"/>
+      <c r="AP25">
+        <v>20</v>
+      </c>
+      <c r="AQ25">
+        <v>20</v>
+      </c>
+      <c r="AR25">
+        <v>40</v>
+      </c>
+      <c r="AS25">
+        <v>40</v>
+      </c>
+      <c r="AT25">
+        <v>40</v>
+      </c>
+      <c r="AU25">
+        <v>40</v>
+      </c>
+      <c r="AV25">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="26" ht="19.5">
-      <c s="6" r="G26"/>
+      <c t="s" r="A26">
+        <v>6</v>
+      </c>
+      <c t="s" r="C26">
+        <v>17</v>
+      </c>
+      <c t="s" r="D26">
+        <v>26</v>
+      </c>
+      <c t="s" r="E26">
+        <v>28</v>
+      </c>
+      <c t="s" r="F26">
+        <v>16</v>
+      </c>
+      <c s="5" r="G26"/>
+      <c r="AP26">
+        <v>20</v>
+      </c>
+      <c r="AQ26">
+        <v>20</v>
+      </c>
+      <c r="AR26">
+        <v>40</v>
+      </c>
+      <c r="AS26">
+        <v>40</v>
+      </c>
+      <c r="AT26">
+        <v>40</v>
+      </c>
+      <c r="AU26">
+        <v>40</v>
+      </c>
+      <c r="AV26">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="27" ht="19.5">
-      <c s="6" r="G27"/>
+      <c t="s" r="A27">
+        <v>6</v>
+      </c>
+      <c t="s" r="C27">
+        <v>19</v>
+      </c>
+      <c t="s" r="D27">
+        <v>26</v>
+      </c>
+      <c t="s" r="E27">
+        <v>28</v>
+      </c>
+      <c t="s" r="F27">
+        <v>10</v>
+      </c>
+      <c s="5" r="G27"/>
+      <c r="AP27">
+        <v>20</v>
+      </c>
+      <c r="AQ27">
+        <v>20</v>
+      </c>
+      <c r="AR27">
+        <v>40</v>
+      </c>
+      <c r="AS27">
+        <v>40</v>
+      </c>
+      <c r="AT27">
+        <v>40</v>
+      </c>
+      <c r="AU27">
+        <v>40</v>
+      </c>
+      <c r="AV27">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="28" ht="19.5">
-      <c s="6" r="G28"/>
+      <c t="s" r="A28">
+        <v>6</v>
+      </c>
+      <c t="s" r="C28">
+        <v>20</v>
+      </c>
+      <c t="s" r="D28">
+        <v>26</v>
+      </c>
+      <c t="s" r="E28">
+        <v>28</v>
+      </c>
+      <c t="s" r="F28">
+        <v>10</v>
+      </c>
+      <c s="5" r="G28"/>
+      <c r="AP28">
+        <v>20</v>
+      </c>
+      <c r="AQ28">
+        <v>20</v>
+      </c>
+      <c r="AR28">
+        <v>40</v>
+      </c>
+      <c r="AS28">
+        <v>40</v>
+      </c>
+      <c r="AT28">
+        <v>40</v>
+      </c>
+      <c r="AU28">
+        <v>40</v>
+      </c>
+      <c r="AV28">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="29" ht="19.5">
-      <c s="6" r="G29"/>
+      <c t="s" r="A29">
+        <v>6</v>
+      </c>
+      <c t="s" r="C29">
+        <v>13</v>
+      </c>
+      <c t="s" r="D29">
+        <v>29</v>
+      </c>
+      <c t="s" r="E29">
+        <v>30</v>
+      </c>
+      <c t="s" r="F29">
+        <v>14</v>
+      </c>
+      <c s="5" r="G29"/>
+      <c r="H29">
+        <v>40</v>
+      </c>
+      <c r="I29">
+        <v>40</v>
+      </c>
+      <c r="J29">
+        <v>40</v>
+      </c>
+      <c r="K29">
+        <v>40</v>
+      </c>
+      <c r="L29">
+        <v>40</v>
+      </c>
+      <c r="M29">
+        <v>40</v>
+      </c>
+      <c r="N29">
+        <v>40</v>
+      </c>
+      <c r="O29">
+        <v>40</v>
+      </c>
+      <c r="P29">
+        <v>40</v>
+      </c>
+      <c r="Q29">
+        <v>40</v>
+      </c>
+      <c r="R29">
+        <v>40</v>
+      </c>
+      <c r="S29">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="30" ht="19.5">
-      <c s="6" r="G30"/>
+      <c t="s" r="A30">
+        <v>6</v>
+      </c>
+      <c t="s" r="C30">
+        <v>15</v>
+      </c>
+      <c t="s" r="D30">
+        <v>29</v>
+      </c>
+      <c t="s" r="E30">
+        <v>30</v>
+      </c>
+      <c t="s" r="F30">
+        <v>16</v>
+      </c>
+      <c s="5" r="G30"/>
+      <c r="H30">
+        <v>40</v>
+      </c>
+      <c r="I30">
+        <v>40</v>
+      </c>
+      <c r="J30">
+        <v>40</v>
+      </c>
+      <c r="K30">
+        <v>40</v>
+      </c>
+      <c r="L30">
+        <v>40</v>
+      </c>
+      <c r="M30">
+        <v>40</v>
+      </c>
+      <c r="N30">
+        <v>40</v>
+      </c>
+      <c r="O30">
+        <v>40</v>
+      </c>
+      <c r="P30">
+        <v>40</v>
+      </c>
+      <c r="Q30">
+        <v>40</v>
+      </c>
+      <c r="R30">
+        <v>40</v>
+      </c>
+      <c r="S30">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="31" ht="19.5">
-      <c s="6" r="G31"/>
+      <c t="s" r="A31">
+        <v>6</v>
+      </c>
+      <c t="s" r="C31">
+        <v>17</v>
+      </c>
+      <c t="s" r="D31">
+        <v>29</v>
+      </c>
+      <c t="s" r="E31">
+        <v>30</v>
+      </c>
+      <c t="s" r="F31">
+        <v>16</v>
+      </c>
+      <c s="5" r="G31"/>
+      <c r="H31">
+        <v>40</v>
+      </c>
+      <c r="I31">
+        <v>40</v>
+      </c>
+      <c r="J31">
+        <v>40</v>
+      </c>
+      <c r="K31">
+        <v>40</v>
+      </c>
+      <c r="L31">
+        <v>40</v>
+      </c>
+      <c r="M31">
+        <v>40</v>
+      </c>
+      <c r="N31">
+        <v>40</v>
+      </c>
+      <c r="O31">
+        <v>40</v>
+      </c>
+      <c r="P31">
+        <v>40</v>
+      </c>
+      <c r="Q31">
+        <v>40</v>
+      </c>
+      <c r="R31">
+        <v>40</v>
+      </c>
+      <c r="S31">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="32" ht="19.5">
-      <c s="6" r="G32"/>
+      <c t="s" r="A32">
+        <v>6</v>
+      </c>
+      <c t="s" r="C32">
+        <v>19</v>
+      </c>
+      <c t="s" r="D32">
+        <v>29</v>
+      </c>
+      <c t="s" r="E32">
+        <v>30</v>
+      </c>
+      <c t="s" r="F32">
+        <v>10</v>
+      </c>
+      <c s="5" r="G32"/>
+      <c r="H32">
+        <v>40</v>
+      </c>
+      <c r="I32">
+        <v>40</v>
+      </c>
+      <c r="J32">
+        <v>40</v>
+      </c>
+      <c r="K32">
+        <v>40</v>
+      </c>
+      <c r="L32">
+        <v>40</v>
+      </c>
+      <c r="M32">
+        <v>40</v>
+      </c>
+      <c r="N32">
+        <v>40</v>
+      </c>
+      <c r="O32">
+        <v>40</v>
+      </c>
+      <c r="P32">
+        <v>40</v>
+      </c>
+      <c r="Q32">
+        <v>40</v>
+      </c>
+      <c r="R32">
+        <v>40</v>
+      </c>
+      <c r="S32">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="33" ht="19.5">
-      <c s="6" r="G33"/>
+      <c t="s" r="A33">
+        <v>6</v>
+      </c>
+      <c t="s" r="C33">
+        <v>20</v>
+      </c>
+      <c t="s" r="D33">
+        <v>29</v>
+      </c>
+      <c t="s" r="E33">
+        <v>30</v>
+      </c>
+      <c t="s" r="F33">
+        <v>10</v>
+      </c>
+      <c s="5" r="G33"/>
+      <c r="H33">
+        <v>40</v>
+      </c>
+      <c r="I33">
+        <v>40</v>
+      </c>
+      <c r="J33">
+        <v>40</v>
+      </c>
+      <c r="K33">
+        <v>40</v>
+      </c>
+      <c r="L33">
+        <v>40</v>
+      </c>
+      <c r="M33">
+        <v>40</v>
+      </c>
+      <c r="N33">
+        <v>40</v>
+      </c>
+      <c r="O33">
+        <v>40</v>
+      </c>
+      <c r="P33">
+        <v>40</v>
+      </c>
+      <c r="Q33">
+        <v>40</v>
+      </c>
+      <c r="R33">
+        <v>40</v>
+      </c>
+      <c r="S33">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="34" ht="19.5">
-      <c s="6" r="G34"/>
+      <c t="s" r="A34">
+        <v>6</v>
+      </c>
+      <c t="s" r="C34">
+        <v>13</v>
+      </c>
+      <c t="s" r="D34">
+        <v>31</v>
+      </c>
+      <c t="s" r="E34">
+        <v>32</v>
+      </c>
+      <c t="s" r="F34">
+        <v>14</v>
+      </c>
+      <c s="5" r="G34"/>
+      <c r="AC34">
+        <v>40</v>
+      </c>
+      <c r="AD34">
+        <v>40</v>
+      </c>
+      <c r="AE34">
+        <v>40</v>
+      </c>
+      <c r="AF34">
+        <v>40</v>
+      </c>
+      <c r="AG34">
+        <v>40</v>
+      </c>
+      <c r="AH34">
+        <v>40</v>
+      </c>
+      <c r="AI34">
+        <v>40</v>
+      </c>
+      <c r="AJ34">
+        <v>40</v>
+      </c>
+      <c r="AK34">
+        <v>40</v>
+      </c>
+      <c r="AL34">
+        <v>40</v>
+      </c>
+      <c r="AM34">
+        <v>40</v>
+      </c>
+      <c r="AN34">
+        <v>40</v>
+      </c>
+      <c r="AO34">
+        <v>40</v>
+      </c>
+      <c r="AP34">
+        <v>40</v>
+      </c>
+      <c r="AQ34">
+        <v>40</v>
+      </c>
+      <c r="AR34">
+        <v>40</v>
+      </c>
+      <c r="AS34">
+        <v>40</v>
+      </c>
+      <c r="AT34">
+        <v>40</v>
+      </c>
+      <c r="AU34">
+        <v>40</v>
+      </c>
+      <c r="AV34">
+        <v>40</v>
+      </c>
+      <c r="AW34">
+        <v>40</v>
+      </c>
+      <c r="AX34">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="35" ht="19.5">
-      <c s="6" r="G35"/>
+      <c t="s" r="A35">
+        <v>6</v>
+      </c>
+      <c t="s" r="C35">
+        <v>15</v>
+      </c>
+      <c t="s" r="D35">
+        <v>31</v>
+      </c>
+      <c t="s" r="E35">
+        <v>32</v>
+      </c>
+      <c t="s" r="F35">
+        <v>16</v>
+      </c>
+      <c s="5" r="G35"/>
+      <c r="AC35">
+        <v>40</v>
+      </c>
+      <c r="AD35">
+        <v>40</v>
+      </c>
+      <c r="AE35">
+        <v>40</v>
+      </c>
+      <c r="AF35">
+        <v>40</v>
+      </c>
+      <c r="AG35">
+        <v>40</v>
+      </c>
+      <c r="AH35">
+        <v>40</v>
+      </c>
+      <c r="AI35">
+        <v>40</v>
+      </c>
+      <c r="AJ35">
+        <v>40</v>
+      </c>
+      <c r="AK35">
+        <v>40</v>
+      </c>
+      <c r="AL35">
+        <v>40</v>
+      </c>
+      <c r="AM35">
+        <v>40</v>
+      </c>
+      <c r="AN35">
+        <v>40</v>
+      </c>
+      <c r="AO35">
+        <v>40</v>
+      </c>
+      <c r="AP35">
+        <v>40</v>
+      </c>
+      <c r="AQ35">
+        <v>40</v>
+      </c>
+      <c r="AR35">
+        <v>40</v>
+      </c>
+      <c r="AS35">
+        <v>40</v>
+      </c>
+      <c r="AT35">
+        <v>40</v>
+      </c>
+      <c r="AU35">
+        <v>40</v>
+      </c>
+      <c r="AV35">
+        <v>40</v>
+      </c>
+      <c r="AW35">
+        <v>40</v>
+      </c>
+      <c r="AX35">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="36" ht="19.5">
-      <c s="6" r="G36"/>
+      <c t="s" r="A36">
+        <v>6</v>
+      </c>
+      <c t="s" r="C36">
+        <v>17</v>
+      </c>
+      <c t="s" r="D36">
+        <v>31</v>
+      </c>
+      <c t="s" r="E36">
+        <v>32</v>
+      </c>
+      <c t="s" r="F36">
+        <v>16</v>
+      </c>
+      <c s="5" r="G36"/>
+      <c r="AC36">
+        <v>40</v>
+      </c>
+      <c r="AD36">
+        <v>40</v>
+      </c>
+      <c r="AE36">
+        <v>40</v>
+      </c>
+      <c r="AF36">
+        <v>40</v>
+      </c>
+      <c r="AG36">
+        <v>40</v>
+      </c>
+      <c r="AH36">
+        <v>40</v>
+      </c>
+      <c r="AI36">
+        <v>40</v>
+      </c>
+      <c r="AJ36">
+        <v>40</v>
+      </c>
+      <c r="AK36">
+        <v>40</v>
+      </c>
+      <c r="AL36">
+        <v>40</v>
+      </c>
+      <c r="AM36">
+        <v>40</v>
+      </c>
+      <c r="AN36">
+        <v>40</v>
+      </c>
+      <c r="AO36">
+        <v>40</v>
+      </c>
+      <c r="AP36">
+        <v>40</v>
+      </c>
+      <c r="AQ36">
+        <v>40</v>
+      </c>
+      <c r="AR36">
+        <v>40</v>
+      </c>
+      <c r="AS36">
+        <v>40</v>
+      </c>
+      <c r="AT36">
+        <v>40</v>
+      </c>
+      <c r="AU36">
+        <v>40</v>
+      </c>
+      <c r="AV36">
+        <v>40</v>
+      </c>
+      <c r="AW36">
+        <v>40</v>
+      </c>
+      <c r="AX36">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="37" ht="19.5">
-      <c s="6" r="G37"/>
+      <c t="s" r="A37">
+        <v>6</v>
+      </c>
+      <c t="s" r="C37">
+        <v>19</v>
+      </c>
+      <c t="s" r="D37">
+        <v>31</v>
+      </c>
+      <c t="s" r="E37">
+        <v>32</v>
+      </c>
+      <c t="s" r="F37">
+        <v>10</v>
+      </c>
+      <c s="5" r="G37"/>
+      <c r="AC37">
+        <v>40</v>
+      </c>
+      <c r="AD37">
+        <v>40</v>
+      </c>
+      <c r="AE37">
+        <v>40</v>
+      </c>
+      <c r="AF37">
+        <v>40</v>
+      </c>
+      <c r="AG37">
+        <v>40</v>
+      </c>
+      <c r="AH37">
+        <v>40</v>
+      </c>
+      <c r="AI37">
+        <v>40</v>
+      </c>
+      <c r="AJ37">
+        <v>40</v>
+      </c>
+      <c r="AK37">
+        <v>40</v>
+      </c>
+      <c r="AL37">
+        <v>40</v>
+      </c>
+      <c r="AM37">
+        <v>40</v>
+      </c>
+      <c r="AN37">
+        <v>40</v>
+      </c>
+      <c r="AO37">
+        <v>40</v>
+      </c>
+      <c r="AP37">
+        <v>40</v>
+      </c>
+      <c r="AQ37">
+        <v>40</v>
+      </c>
+      <c r="AR37">
+        <v>40</v>
+      </c>
+      <c r="AS37">
+        <v>40</v>
+      </c>
+      <c r="AT37">
+        <v>40</v>
+      </c>
+      <c r="AU37">
+        <v>40</v>
+      </c>
+      <c r="AV37">
+        <v>40</v>
+      </c>
+      <c r="AW37">
+        <v>40</v>
+      </c>
+      <c r="AX37">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="38" ht="19.5">
-      <c s="6" r="G38"/>
+      <c t="s" r="A38">
+        <v>6</v>
+      </c>
+      <c t="s" r="C38">
+        <v>20</v>
+      </c>
+      <c t="s" r="D38">
+        <v>31</v>
+      </c>
+      <c t="s" r="E38">
+        <v>32</v>
+      </c>
+      <c t="s" r="F38">
+        <v>10</v>
+      </c>
+      <c s="5" r="G38"/>
+      <c r="AC38">
+        <v>40</v>
+      </c>
+      <c r="AD38">
+        <v>40</v>
+      </c>
+      <c r="AE38">
+        <v>40</v>
+      </c>
+      <c r="AF38">
+        <v>40</v>
+      </c>
+      <c r="AG38">
+        <v>40</v>
+      </c>
+      <c r="AH38">
+        <v>40</v>
+      </c>
+      <c r="AI38">
+        <v>40</v>
+      </c>
+      <c r="AJ38">
+        <v>40</v>
+      </c>
+      <c r="AK38">
+        <v>40</v>
+      </c>
+      <c r="AL38">
+        <v>40</v>
+      </c>
+      <c r="AM38">
+        <v>40</v>
+      </c>
+      <c r="AN38">
+        <v>40</v>
+      </c>
+      <c r="AO38">
+        <v>40</v>
+      </c>
+      <c r="AP38">
+        <v>40</v>
+      </c>
+      <c r="AQ38">
+        <v>40</v>
+      </c>
+      <c r="AR38">
+        <v>40</v>
+      </c>
+      <c r="AS38">
+        <v>40</v>
+      </c>
+      <c r="AT38">
+        <v>40</v>
+      </c>
+      <c r="AU38">
+        <v>40</v>
+      </c>
+      <c r="AV38">
+        <v>40</v>
+      </c>
+      <c r="AW38">
+        <v>40</v>
+      </c>
+      <c r="AX38">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="39" ht="19.5">
-      <c s="6" r="G39"/>
+      <c t="s" r="A39">
+        <v>6</v>
+      </c>
+      <c t="s" r="C39">
+        <v>13</v>
+      </c>
+      <c t="s" r="D39">
+        <v>31</v>
+      </c>
+      <c t="s" r="E39">
+        <v>33</v>
+      </c>
+      <c t="s" r="F39">
+        <v>14</v>
+      </c>
+      <c s="5" r="G39"/>
+      <c r="BD39">
+        <v>40</v>
+      </c>
+      <c r="BE39">
+        <v>40</v>
+      </c>
+      <c r="BF39">
+        <v>40</v>
+      </c>
+      <c r="BG39">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="40" ht="19.5">
-      <c s="6" r="G40"/>
+      <c t="s" r="A40">
+        <v>6</v>
+      </c>
+      <c t="s" r="C40">
+        <v>15</v>
+      </c>
+      <c t="s" r="D40">
+        <v>31</v>
+      </c>
+      <c t="s" r="E40">
+        <v>33</v>
+      </c>
+      <c t="s" r="F40">
+        <v>16</v>
+      </c>
+      <c s="5" r="G40"/>
+      <c r="BD40">
+        <v>40</v>
+      </c>
+      <c r="BE40">
+        <v>40</v>
+      </c>
+      <c r="BF40">
+        <v>40</v>
+      </c>
+      <c r="BG40">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="41" ht="19.5">
-      <c s="6" r="G41"/>
+      <c t="s" r="A41">
+        <v>6</v>
+      </c>
+      <c t="s" r="C41">
+        <v>17</v>
+      </c>
+      <c t="s" r="D41">
+        <v>31</v>
+      </c>
+      <c t="s" r="E41">
+        <v>33</v>
+      </c>
+      <c t="s" r="F41">
+        <v>16</v>
+      </c>
+      <c s="5" r="G41"/>
+      <c r="BD41">
+        <v>40</v>
+      </c>
+      <c r="BE41">
+        <v>40</v>
+      </c>
+      <c r="BF41">
+        <v>40</v>
+      </c>
+      <c r="BG41">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="42" ht="19.5">
-      <c s="6" r="G42"/>
+      <c t="s" r="A42">
+        <v>6</v>
+      </c>
+      <c t="s" r="C42">
+        <v>19</v>
+      </c>
+      <c t="s" r="D42">
+        <v>31</v>
+      </c>
+      <c t="s" r="E42">
+        <v>33</v>
+      </c>
+      <c t="s" r="F42">
+        <v>10</v>
+      </c>
+      <c s="5" r="G42"/>
+      <c r="BD42">
+        <v>40</v>
+      </c>
+      <c r="BE42">
+        <v>40</v>
+      </c>
+      <c r="BF42">
+        <v>40</v>
+      </c>
+      <c r="BG42">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="43" ht="19.5">
-      <c s="6" r="G43"/>
+      <c t="s" r="A43">
+        <v>6</v>
+      </c>
+      <c t="s" r="C43">
+        <v>20</v>
+      </c>
+      <c t="s" r="D43">
+        <v>31</v>
+      </c>
+      <c t="s" r="E43">
+        <v>33</v>
+      </c>
+      <c t="s" r="F43">
+        <v>10</v>
+      </c>
+      <c s="5" r="G43"/>
+      <c r="BD43">
+        <v>40</v>
+      </c>
+      <c r="BE43">
+        <v>40</v>
+      </c>
+      <c r="BF43">
+        <v>40</v>
+      </c>
+      <c r="BG43">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="44" ht="19.5">
-      <c s="6" r="G44"/>
+      <c t="s" r="A44">
+        <v>6</v>
+      </c>
+      <c t="s" r="C44">
+        <v>13</v>
+      </c>
+      <c t="s" r="D44">
+        <v>34</v>
+      </c>
+      <c t="s" r="E44">
+        <v>35</v>
+      </c>
+      <c t="s" r="F44">
+        <v>14</v>
+      </c>
+      <c s="5" r="G44"/>
+      <c r="Q44">
+        <v>40</v>
+      </c>
+      <c r="R44">
+        <v>40</v>
+      </c>
+      <c r="S44">
+        <v>40</v>
+      </c>
+      <c r="T44">
+        <v>40</v>
+      </c>
+      <c r="U44">
+        <v>40</v>
+      </c>
+      <c r="V44">
+        <v>40</v>
+      </c>
+      <c r="W44">
+        <v>40</v>
+      </c>
+      <c r="X44">
+        <v>40</v>
+      </c>
+      <c r="Y44">
+        <v>40</v>
+      </c>
+      <c r="Z44">
+        <v>40</v>
+      </c>
+      <c r="AA44">
+        <v>40</v>
+      </c>
+      <c r="AB44">
+        <v>40</v>
+      </c>
+      <c r="AC44">
+        <v>40</v>
+      </c>
+      <c r="AD44">
+        <v>40</v>
+      </c>
+      <c r="AE44">
+        <v>40</v>
+      </c>
+      <c r="AF44">
+        <v>40</v>
+      </c>
+      <c r="AG44">
+        <v>40</v>
+      </c>
+      <c r="AH44">
+        <v>40</v>
+      </c>
+      <c r="AI44">
+        <v>40</v>
+      </c>
+      <c r="AJ44">
+        <v>40</v>
+      </c>
+      <c r="AK44">
+        <v>24</v>
+      </c>
     </row>
     <row customHeight="1" r="45" ht="19.5">
-      <c s="6" r="G45"/>
+      <c t="s" r="A45">
+        <v>6</v>
+      </c>
+      <c t="s" r="C45">
+        <v>15</v>
+      </c>
+      <c t="s" r="D45">
+        <v>34</v>
+      </c>
+      <c t="s" r="E45">
+        <v>35</v>
+      </c>
+      <c t="s" r="F45">
+        <v>16</v>
+      </c>
+      <c s="5" r="G45"/>
+      <c r="Q45">
+        <v>40</v>
+      </c>
+      <c r="R45">
+        <v>40</v>
+      </c>
+      <c r="S45">
+        <v>40</v>
+      </c>
+      <c r="T45">
+        <v>40</v>
+      </c>
+      <c r="U45">
+        <v>40</v>
+      </c>
+      <c r="V45">
+        <v>40</v>
+      </c>
+      <c r="W45">
+        <v>40</v>
+      </c>
+      <c r="X45">
+        <v>40</v>
+      </c>
+      <c r="Y45">
+        <v>40</v>
+      </c>
+      <c r="Z45">
+        <v>40</v>
+      </c>
+      <c r="AA45">
+        <v>40</v>
+      </c>
+      <c r="AB45">
+        <v>40</v>
+      </c>
+      <c r="AC45">
+        <v>40</v>
+      </c>
+      <c r="AD45">
+        <v>40</v>
+      </c>
+      <c r="AE45">
+        <v>40</v>
+      </c>
+      <c r="AF45">
+        <v>40</v>
+      </c>
+      <c r="AG45">
+        <v>40</v>
+      </c>
+      <c r="AH45">
+        <v>40</v>
+      </c>
+      <c r="AI45">
+        <v>40</v>
+      </c>
+      <c r="AJ45">
+        <v>40</v>
+      </c>
+      <c r="AK45">
+        <v>24</v>
+      </c>
     </row>
     <row customHeight="1" r="46" ht="19.5">
-      <c s="6" r="G46"/>
+      <c t="s" r="A46">
+        <v>6</v>
+      </c>
+      <c t="s" r="C46">
+        <v>17</v>
+      </c>
+      <c t="s" r="D46">
+        <v>34</v>
+      </c>
+      <c t="s" r="E46">
+        <v>35</v>
+      </c>
+      <c t="s" r="F46">
+        <v>16</v>
+      </c>
+      <c s="5" r="G46"/>
+      <c r="Q46">
+        <v>40</v>
+      </c>
+      <c r="R46">
+        <v>40</v>
+      </c>
+      <c r="S46">
+        <v>40</v>
+      </c>
+      <c r="T46">
+        <v>40</v>
+      </c>
+      <c r="U46">
+        <v>40</v>
+      </c>
+      <c r="V46">
+        <v>40</v>
+      </c>
+      <c r="W46">
+        <v>40</v>
+      </c>
+      <c r="X46">
+        <v>40</v>
+      </c>
+      <c r="Y46">
+        <v>40</v>
+      </c>
+      <c r="Z46">
+        <v>40</v>
+      </c>
+      <c r="AA46">
+        <v>40</v>
+      </c>
+      <c r="AB46">
+        <v>40</v>
+      </c>
+      <c r="AC46">
+        <v>40</v>
+      </c>
+      <c r="AD46">
+        <v>40</v>
+      </c>
+      <c r="AE46">
+        <v>40</v>
+      </c>
+      <c r="AF46">
+        <v>40</v>
+      </c>
+      <c r="AG46">
+        <v>40</v>
+      </c>
+      <c r="AH46">
+        <v>40</v>
+      </c>
+      <c r="AI46">
+        <v>40</v>
+      </c>
+      <c r="AJ46">
+        <v>40</v>
+      </c>
+      <c r="AK46">
+        <v>24</v>
+      </c>
     </row>
     <row customHeight="1" r="47" ht="19.5">
-      <c s="6" r="G47"/>
+      <c t="s" r="A47">
+        <v>6</v>
+      </c>
+      <c t="s" r="C47">
+        <v>19</v>
+      </c>
+      <c t="s" r="D47">
+        <v>34</v>
+      </c>
+      <c t="s" r="E47">
+        <v>35</v>
+      </c>
+      <c t="s" r="F47">
+        <v>10</v>
+      </c>
+      <c s="5" r="G47"/>
+      <c r="Q47">
+        <v>40</v>
+      </c>
+      <c r="R47">
+        <v>40</v>
+      </c>
+      <c r="S47">
+        <v>40</v>
+      </c>
+      <c r="T47">
+        <v>40</v>
+      </c>
+      <c r="U47">
+        <v>40</v>
+      </c>
+      <c r="V47">
+        <v>40</v>
+      </c>
+      <c r="W47">
+        <v>40</v>
+      </c>
+      <c r="X47">
+        <v>40</v>
+      </c>
+      <c r="Y47">
+        <v>40</v>
+      </c>
+      <c r="Z47">
+        <v>40</v>
+      </c>
+      <c r="AA47">
+        <v>40</v>
+      </c>
+      <c r="AB47">
+        <v>40</v>
+      </c>
+      <c r="AC47">
+        <v>40</v>
+      </c>
+      <c r="AD47">
+        <v>40</v>
+      </c>
+      <c r="AE47">
+        <v>40</v>
+      </c>
+      <c r="AF47">
+        <v>40</v>
+      </c>
+      <c r="AG47">
+        <v>40</v>
+      </c>
+      <c r="AH47">
+        <v>40</v>
+      </c>
+      <c r="AI47">
+        <v>40</v>
+      </c>
+      <c r="AJ47">
+        <v>40</v>
+      </c>
+      <c r="AK47">
+        <v>24</v>
+      </c>
     </row>
     <row customHeight="1" r="48" ht="19.5">
-      <c s="6" r="G48"/>
+      <c t="s" r="A48">
+        <v>6</v>
+      </c>
+      <c t="s" r="C48">
+        <v>20</v>
+      </c>
+      <c t="s" r="D48">
+        <v>34</v>
+      </c>
+      <c t="s" r="E48">
+        <v>35</v>
+      </c>
+      <c t="s" r="F48">
+        <v>10</v>
+      </c>
+      <c s="5" r="G48"/>
+      <c r="Q48">
+        <v>40</v>
+      </c>
+      <c r="R48">
+        <v>40</v>
+      </c>
+      <c r="S48">
+        <v>40</v>
+      </c>
+      <c r="T48">
+        <v>40</v>
+      </c>
+      <c r="U48">
+        <v>40</v>
+      </c>
+      <c r="V48">
+        <v>40</v>
+      </c>
+      <c r="W48">
+        <v>40</v>
+      </c>
+      <c r="X48">
+        <v>40</v>
+      </c>
+      <c r="Y48">
+        <v>40</v>
+      </c>
+      <c r="Z48">
+        <v>40</v>
+      </c>
+      <c r="AA48">
+        <v>40</v>
+      </c>
+      <c r="AB48">
+        <v>40</v>
+      </c>
+      <c r="AC48">
+        <v>40</v>
+      </c>
+      <c r="AD48">
+        <v>40</v>
+      </c>
+      <c r="AE48">
+        <v>40</v>
+      </c>
+      <c r="AF48">
+        <v>40</v>
+      </c>
+      <c r="AG48">
+        <v>40</v>
+      </c>
+      <c r="AH48">
+        <v>40</v>
+      </c>
+      <c r="AI48">
+        <v>40</v>
+      </c>
+      <c r="AJ48">
+        <v>40</v>
+      </c>
+      <c r="AK48">
+        <v>24</v>
+      </c>
     </row>
     <row customHeight="1" r="49" ht="19.5">
-      <c s="6" r="G49"/>
+      <c t="s" r="A49">
+        <v>6</v>
+      </c>
+      <c t="s" r="C49">
+        <v>13</v>
+      </c>
+      <c t="s" r="D49">
+        <v>36</v>
+      </c>
+      <c t="s" r="E49">
+        <v>30</v>
+      </c>
+      <c t="s" r="F49">
+        <v>14</v>
+      </c>
+      <c s="5" r="G49"/>
+      <c r="AO49">
+        <v>40</v>
+      </c>
+      <c r="AP49">
+        <v>40</v>
+      </c>
+      <c r="AQ49">
+        <v>40</v>
+      </c>
+      <c r="AR49">
+        <v>40</v>
+      </c>
+      <c r="AS49">
+        <v>40</v>
+      </c>
+      <c r="AT49">
+        <v>40</v>
+      </c>
+      <c r="AU49">
+        <v>40</v>
+      </c>
+      <c r="AV49">
+        <v>40</v>
+      </c>
+      <c r="AW49">
+        <v>40</v>
+      </c>
+      <c r="AX49">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="50" ht="19.5">
-      <c s="6" r="G50"/>
+      <c t="s" r="A50">
+        <v>6</v>
+      </c>
+      <c t="s" r="C50">
+        <v>15</v>
+      </c>
+      <c t="s" r="D50">
+        <v>36</v>
+      </c>
+      <c t="s" r="E50">
+        <v>30</v>
+      </c>
+      <c t="s" r="F50">
+        <v>16</v>
+      </c>
+      <c s="5" r="G50"/>
+      <c r="AO50">
+        <v>40</v>
+      </c>
+      <c r="AP50">
+        <v>40</v>
+      </c>
+      <c r="AQ50">
+        <v>40</v>
+      </c>
+      <c r="AR50">
+        <v>40</v>
+      </c>
+      <c r="AS50">
+        <v>40</v>
+      </c>
+      <c r="AT50">
+        <v>40</v>
+      </c>
+      <c r="AU50">
+        <v>40</v>
+      </c>
+      <c r="AV50">
+        <v>40</v>
+      </c>
+      <c r="AW50">
+        <v>40</v>
+      </c>
+      <c r="AX50">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="51" ht="19.5">
-      <c s="6" r="G51"/>
+      <c t="s" r="A51">
+        <v>6</v>
+      </c>
+      <c t="s" r="C51">
+        <v>17</v>
+      </c>
+      <c t="s" r="D51">
+        <v>36</v>
+      </c>
+      <c t="s" r="E51">
+        <v>30</v>
+      </c>
+      <c t="s" r="F51">
+        <v>16</v>
+      </c>
+      <c s="5" r="G51"/>
+      <c r="AO51">
+        <v>40</v>
+      </c>
+      <c r="AP51">
+        <v>40</v>
+      </c>
+      <c r="AQ51">
+        <v>40</v>
+      </c>
+      <c r="AR51">
+        <v>40</v>
+      </c>
+      <c r="AS51">
+        <v>40</v>
+      </c>
+      <c r="AT51">
+        <v>40</v>
+      </c>
+      <c r="AU51">
+        <v>40</v>
+      </c>
+      <c r="AV51">
+        <v>40</v>
+      </c>
+      <c r="AW51">
+        <v>40</v>
+      </c>
+      <c r="AX51">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="52" ht="19.5">
-      <c s="6" r="G52"/>
+      <c t="s" r="A52">
+        <v>6</v>
+      </c>
+      <c t="s" r="C52">
+        <v>19</v>
+      </c>
+      <c t="s" r="D52">
+        <v>36</v>
+      </c>
+      <c t="s" r="E52">
+        <v>30</v>
+      </c>
+      <c t="s" r="F52">
+        <v>10</v>
+      </c>
+      <c s="5" r="G52"/>
+      <c r="AO52">
+        <v>40</v>
+      </c>
+      <c r="AP52">
+        <v>40</v>
+      </c>
+      <c r="AQ52">
+        <v>40</v>
+      </c>
+      <c r="AR52">
+        <v>40</v>
+      </c>
+      <c r="AS52">
+        <v>40</v>
+      </c>
+      <c r="AT52">
+        <v>40</v>
+      </c>
+      <c r="AU52">
+        <v>40</v>
+      </c>
+      <c r="AV52">
+        <v>40</v>
+      </c>
+      <c r="AW52">
+        <v>40</v>
+      </c>
+      <c r="AX52">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="53" ht="19.5">
-      <c s="6" r="G53"/>
+      <c t="s" r="A53">
+        <v>6</v>
+      </c>
+      <c t="s" r="C53">
+        <v>20</v>
+      </c>
+      <c t="s" r="D53">
+        <v>36</v>
+      </c>
+      <c t="s" r="E53">
+        <v>30</v>
+      </c>
+      <c t="s" r="F53">
+        <v>10</v>
+      </c>
+      <c s="5" r="G53"/>
+      <c r="AO53">
+        <v>40</v>
+      </c>
+      <c r="AP53">
+        <v>40</v>
+      </c>
+      <c r="AQ53">
+        <v>40</v>
+      </c>
+      <c r="AR53">
+        <v>40</v>
+      </c>
+      <c r="AS53">
+        <v>40</v>
+      </c>
+      <c r="AT53">
+        <v>40</v>
+      </c>
+      <c r="AU53">
+        <v>40</v>
+      </c>
+      <c r="AV53">
+        <v>40</v>
+      </c>
+      <c r="AW53">
+        <v>40</v>
+      </c>
+      <c r="AX53">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" r="54" ht="19.5">
-      <c s="6" r="G54"/>
+      <c t="s" r="A54">
+        <v>6</v>
+      </c>
+      <c t="s" r="C54">
+        <v>13</v>
+      </c>
+      <c t="s" r="D54">
+        <v>37</v>
+      </c>
+      <c t="s" r="E54">
+        <v>38</v>
+      </c>
+      <c t="s" r="F54">
+        <v>14</v>
+      </c>
+      <c s="5" r="G54"/>
+      <c r="H54">
+        <v>12</v>
+      </c>
+      <c r="I54">
+        <v>12</v>
+      </c>
+      <c r="J54">
+        <v>12</v>
+      </c>
+      <c r="K54">
+        <v>12</v>
+      </c>
+      <c r="L54">
+        <v>12</v>
+      </c>
+      <c r="M54">
+        <v>12</v>
+      </c>
+      <c r="N54">
+        <v>12</v>
+      </c>
+      <c r="O54">
+        <v>12</v>
+      </c>
+      <c r="P54">
+        <v>12</v>
+      </c>
+      <c r="Q54">
+        <v>12</v>
+      </c>
+      <c r="R54">
+        <v>12</v>
+      </c>
+      <c r="S54">
+        <v>12</v>
+      </c>
+      <c r="T54">
+        <v>12</v>
+      </c>
+      <c r="AH54">
+        <v>12</v>
+      </c>
+      <c r="AI54">
+        <v>12</v>
+      </c>
+      <c r="AJ54">
+        <v>12</v>
+      </c>
+      <c r="AK54">
+        <v>12</v>
+      </c>
+      <c r="AL54">
+        <v>12</v>
+      </c>
+      <c r="AM54">
+        <v>12</v>
+      </c>
+      <c r="AN54">
+        <v>12</v>
+      </c>
+      <c r="AO54">
+        <v>12</v>
+      </c>
+      <c r="AP54">
+        <v>12</v>
+      </c>
+      <c r="BD54">
+        <v>12</v>
+      </c>
+      <c r="BE54">
+        <v>12</v>
+      </c>
+      <c r="BF54">
+        <v>12</v>
+      </c>
+      <c r="BG54">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="55" ht="19.5">
-      <c s="6" r="G55"/>
+      <c t="s" r="A55">
+        <v>6</v>
+      </c>
+      <c t="s" r="C55">
+        <v>15</v>
+      </c>
+      <c t="s" r="D55">
+        <v>37</v>
+      </c>
+      <c t="s" r="E55">
+        <v>38</v>
+      </c>
+      <c t="s" r="F55">
+        <v>16</v>
+      </c>
+      <c s="5" r="G55"/>
+      <c r="H55">
+        <v>12</v>
+      </c>
+      <c r="I55">
+        <v>12</v>
+      </c>
+      <c r="J55">
+        <v>12</v>
+      </c>
+      <c r="K55">
+        <v>12</v>
+      </c>
+      <c r="L55">
+        <v>12</v>
+      </c>
+      <c r="M55">
+        <v>12</v>
+      </c>
+      <c r="N55">
+        <v>12</v>
+      </c>
+      <c r="O55">
+        <v>12</v>
+      </c>
+      <c r="P55">
+        <v>12</v>
+      </c>
+      <c r="Q55">
+        <v>12</v>
+      </c>
+      <c r="R55">
+        <v>12</v>
+      </c>
+      <c r="S55">
+        <v>12</v>
+      </c>
+      <c r="T55">
+        <v>12</v>
+      </c>
+      <c r="AH55">
+        <v>12</v>
+      </c>
+      <c r="AI55">
+        <v>12</v>
+      </c>
+      <c r="AJ55">
+        <v>12</v>
+      </c>
+      <c r="AK55">
+        <v>12</v>
+      </c>
+      <c r="AL55">
+        <v>12</v>
+      </c>
+      <c r="AM55">
+        <v>12</v>
+      </c>
+      <c r="AN55">
+        <v>12</v>
+      </c>
+      <c r="AO55">
+        <v>12</v>
+      </c>
+      <c r="AP55">
+        <v>12</v>
+      </c>
+      <c r="BD55">
+        <v>12</v>
+      </c>
+      <c r="BE55">
+        <v>12</v>
+      </c>
+      <c r="BF55">
+        <v>12</v>
+      </c>
+      <c r="BG55">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="56" ht="19.5">
-      <c s="6" r="G56"/>
+      <c t="s" r="A56">
+        <v>6</v>
+      </c>
+      <c t="s" r="C56">
+        <v>17</v>
+      </c>
+      <c t="s" r="D56">
+        <v>37</v>
+      </c>
+      <c t="s" r="E56">
+        <v>38</v>
+      </c>
+      <c t="s" r="F56">
+        <v>16</v>
+      </c>
+      <c s="5" r="G56"/>
+      <c r="H56">
+        <v>12</v>
+      </c>
+      <c r="I56">
+        <v>12</v>
+      </c>
+      <c r="J56">
+        <v>12</v>
+      </c>
+      <c r="K56">
+        <v>12</v>
+      </c>
+      <c r="L56">
+        <v>12</v>
+      </c>
+      <c r="M56">
+        <v>12</v>
+      </c>
+      <c r="N56">
+        <v>12</v>
+      </c>
+      <c r="O56">
+        <v>12</v>
+      </c>
+      <c r="P56">
+        <v>12</v>
+      </c>
+      <c r="Q56">
+        <v>12</v>
+      </c>
+      <c r="R56">
+        <v>12</v>
+      </c>
+      <c r="S56">
+        <v>12</v>
+      </c>
+      <c r="T56">
+        <v>12</v>
+      </c>
+      <c r="AH56">
+        <v>12</v>
+      </c>
+      <c r="AI56">
+        <v>12</v>
+      </c>
+      <c r="AJ56">
+        <v>12</v>
+      </c>
+      <c r="AK56">
+        <v>12</v>
+      </c>
+      <c r="AL56">
+        <v>12</v>
+      </c>
+      <c r="AM56">
+        <v>12</v>
+      </c>
+      <c r="AN56">
+        <v>12</v>
+      </c>
+      <c r="AO56">
+        <v>12</v>
+      </c>
+      <c r="AP56">
+        <v>12</v>
+      </c>
+      <c r="BD56">
+        <v>12</v>
+      </c>
+      <c r="BE56">
+        <v>12</v>
+      </c>
+      <c r="BF56">
+        <v>12</v>
+      </c>
+      <c r="BG56">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="57" ht="19.5">
-      <c s="6" r="G57"/>
+      <c t="s" r="A57">
+        <v>6</v>
+      </c>
+      <c t="s" r="C57">
+        <v>19</v>
+      </c>
+      <c t="s" r="D57">
+        <v>37</v>
+      </c>
+      <c t="s" r="E57">
+        <v>38</v>
+      </c>
+      <c t="s" r="F57">
+        <v>10</v>
+      </c>
+      <c s="5" r="G57"/>
+      <c r="H57">
+        <v>12</v>
+      </c>
+      <c r="I57">
+        <v>12</v>
+      </c>
+      <c r="J57">
+        <v>12</v>
+      </c>
+      <c r="K57">
+        <v>12</v>
+      </c>
+      <c r="L57">
+        <v>12</v>
+      </c>
+      <c r="M57">
+        <v>12</v>
+      </c>
+      <c r="N57">
+        <v>12</v>
+      </c>
+      <c r="O57">
+        <v>12</v>
+      </c>
+      <c r="P57">
+        <v>12</v>
+      </c>
+      <c r="Q57">
+        <v>12</v>
+      </c>
+      <c r="R57">
+        <v>12</v>
+      </c>
+      <c r="S57">
+        <v>12</v>
+      </c>
+      <c r="T57">
+        <v>12</v>
+      </c>
+      <c r="AH57">
+        <v>12</v>
+      </c>
+      <c r="AI57">
+        <v>12</v>
+      </c>
+      <c r="AJ57">
+        <v>12</v>
+      </c>
+      <c r="AK57">
+        <v>12</v>
+      </c>
+      <c r="AL57">
+        <v>12</v>
+      </c>
+      <c r="AM57">
+        <v>12</v>
+      </c>
+      <c r="AN57">
+        <v>12</v>
+      </c>
+      <c r="AO57">
+        <v>12</v>
+      </c>
+      <c r="AP57">
+        <v>12</v>
+      </c>
+      <c r="BD57">
+        <v>12</v>
+      </c>
+      <c r="BE57">
+        <v>12</v>
+      </c>
+      <c r="BF57">
+        <v>12</v>
+      </c>
+      <c r="BG57">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="58" ht="19.5">
-      <c s="6" r="G58"/>
+      <c t="s" r="A58">
+        <v>6</v>
+      </c>
+      <c t="s" r="C58">
+        <v>20</v>
+      </c>
+      <c t="s" r="D58">
+        <v>37</v>
+      </c>
+      <c t="s" r="E58">
+        <v>38</v>
+      </c>
+      <c t="s" r="F58">
+        <v>10</v>
+      </c>
+      <c s="5" r="G58"/>
+      <c r="H58">
+        <v>12</v>
+      </c>
+      <c r="I58">
+        <v>12</v>
+      </c>
+      <c r="J58">
+        <v>12</v>
+      </c>
+      <c r="K58">
+        <v>12</v>
+      </c>
+      <c r="L58">
+        <v>12</v>
+      </c>
+      <c r="M58">
+        <v>12</v>
+      </c>
+      <c r="N58">
+        <v>12</v>
+      </c>
+      <c r="O58">
+        <v>12</v>
+      </c>
+      <c r="P58">
+        <v>12</v>
+      </c>
+      <c r="Q58">
+        <v>12</v>
+      </c>
+      <c r="R58">
+        <v>12</v>
+      </c>
+      <c r="S58">
+        <v>12</v>
+      </c>
+      <c r="T58">
+        <v>12</v>
+      </c>
+      <c r="AH58">
+        <v>12</v>
+      </c>
+      <c r="AI58">
+        <v>12</v>
+      </c>
+      <c r="AJ58">
+        <v>12</v>
+      </c>
+      <c r="AK58">
+        <v>12</v>
+      </c>
+      <c r="AL58">
+        <v>12</v>
+      </c>
+      <c r="AM58">
+        <v>12</v>
+      </c>
+      <c r="AN58">
+        <v>12</v>
+      </c>
+      <c r="AO58">
+        <v>12</v>
+      </c>
+      <c r="AP58">
+        <v>12</v>
+      </c>
+      <c r="BD58">
+        <v>12</v>
+      </c>
+      <c r="BE58">
+        <v>12</v>
+      </c>
+      <c r="BF58">
+        <v>12</v>
+      </c>
+      <c r="BG58">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="59" ht="19.5">
-      <c s="6" r="G59"/>
+      <c t="s" r="A59">
+        <v>6</v>
+      </c>
+      <c t="s" r="C59">
+        <v>13</v>
+      </c>
+      <c t="s" r="D59">
+        <v>39</v>
+      </c>
+      <c t="s" r="E59">
+        <v>40</v>
+      </c>
+      <c t="s" r="F59">
+        <v>14</v>
+      </c>
+      <c s="5" r="G59"/>
+      <c r="U59">
+        <v>12</v>
+      </c>
+      <c r="V59">
+        <v>12</v>
+      </c>
+      <c r="W59">
+        <v>12</v>
+      </c>
+      <c r="X59">
+        <v>12</v>
+      </c>
+      <c r="Y59">
+        <v>12</v>
+      </c>
+      <c r="Z59">
+        <v>12</v>
+      </c>
+      <c r="AA59">
+        <v>12</v>
+      </c>
+      <c r="AB59">
+        <v>12</v>
+      </c>
+      <c r="AC59">
+        <v>12</v>
+      </c>
+      <c r="AD59">
+        <v>12</v>
+      </c>
+      <c r="AE59">
+        <v>12</v>
+      </c>
+      <c r="AF59">
+        <v>12</v>
+      </c>
+      <c r="AG59">
+        <v>12</v>
+      </c>
+      <c r="AQ59">
+        <v>12</v>
+      </c>
+      <c r="AR59">
+        <v>12</v>
+      </c>
+      <c r="AS59">
+        <v>12</v>
+      </c>
+      <c r="AT59">
+        <v>12</v>
+      </c>
+      <c r="AU59">
+        <v>12</v>
+      </c>
+      <c r="AV59">
+        <v>12</v>
+      </c>
+      <c r="AW59">
+        <v>12</v>
+      </c>
+      <c r="AX59">
+        <v>12</v>
+      </c>
+      <c r="AY59">
+        <v>12</v>
+      </c>
+      <c r="AZ59">
+        <v>12</v>
+      </c>
+      <c r="BA59">
+        <v>12</v>
+      </c>
+      <c r="BB59">
+        <v>12</v>
+      </c>
+      <c r="BC59">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="60" ht="19.5">
-      <c s="6" r="G60"/>
+      <c t="s" r="A60">
+        <v>6</v>
+      </c>
+      <c t="s" r="C60">
+        <v>15</v>
+      </c>
+      <c t="s" r="D60">
+        <v>41</v>
+      </c>
+      <c t="s" r="E60">
+        <v>40</v>
+      </c>
+      <c t="s" r="F60">
+        <v>16</v>
+      </c>
+      <c s="5" r="G60"/>
+      <c r="U60">
+        <v>12</v>
+      </c>
+      <c r="V60">
+        <v>12</v>
+      </c>
+      <c r="W60">
+        <v>12</v>
+      </c>
+      <c r="X60">
+        <v>12</v>
+      </c>
+      <c r="Y60">
+        <v>12</v>
+      </c>
+      <c r="Z60">
+        <v>12</v>
+      </c>
+      <c r="AA60">
+        <v>12</v>
+      </c>
+      <c r="AB60">
+        <v>12</v>
+      </c>
+      <c r="AC60">
+        <v>12</v>
+      </c>
+      <c r="AD60">
+        <v>12</v>
+      </c>
+      <c r="AE60">
+        <v>12</v>
+      </c>
+      <c r="AF60">
+        <v>12</v>
+      </c>
+      <c r="AG60">
+        <v>12</v>
+      </c>
+      <c r="AQ60">
+        <v>12</v>
+      </c>
+      <c r="AR60">
+        <v>12</v>
+      </c>
+      <c r="AS60">
+        <v>12</v>
+      </c>
+      <c r="AT60">
+        <v>12</v>
+      </c>
+      <c r="AU60">
+        <v>12</v>
+      </c>
+      <c r="AV60">
+        <v>12</v>
+      </c>
+      <c r="AW60">
+        <v>12</v>
+      </c>
+      <c r="AX60">
+        <v>12</v>
+      </c>
+      <c r="AY60">
+        <v>12</v>
+      </c>
+      <c r="AZ60">
+        <v>12</v>
+      </c>
+      <c r="BA60">
+        <v>12</v>
+      </c>
+      <c r="BB60">
+        <v>12</v>
+      </c>
+      <c r="BC60">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="61" ht="19.5">
-      <c s="6" r="G61"/>
+      <c t="s" r="A61">
+        <v>6</v>
+      </c>
+      <c t="s" r="C61">
+        <v>17</v>
+      </c>
+      <c t="s" r="D61">
+        <v>41</v>
+      </c>
+      <c t="s" r="E61">
+        <v>40</v>
+      </c>
+      <c t="s" r="F61">
+        <v>16</v>
+      </c>
+      <c s="5" r="G61"/>
+      <c r="U61">
+        <v>12</v>
+      </c>
+      <c r="V61">
+        <v>12</v>
+      </c>
+      <c r="W61">
+        <v>12</v>
+      </c>
+      <c r="X61">
+        <v>12</v>
+      </c>
+      <c r="Y61">
+        <v>12</v>
+      </c>
+      <c r="Z61">
+        <v>12</v>
+      </c>
+      <c r="AA61">
+        <v>12</v>
+      </c>
+      <c r="AB61">
+        <v>12</v>
+      </c>
+      <c r="AC61">
+        <v>12</v>
+      </c>
+      <c r="AD61">
+        <v>12</v>
+      </c>
+      <c r="AE61">
+        <v>12</v>
+      </c>
+      <c r="AF61">
+        <v>12</v>
+      </c>
+      <c r="AG61">
+        <v>12</v>
+      </c>
+      <c r="AQ61">
+        <v>12</v>
+      </c>
+      <c r="AR61">
+        <v>12</v>
+      </c>
+      <c r="AS61">
+        <v>12</v>
+      </c>
+      <c r="AT61">
+        <v>12</v>
+      </c>
+      <c r="AU61">
+        <v>12</v>
+      </c>
+      <c r="AV61">
+        <v>12</v>
+      </c>
+      <c r="AW61">
+        <v>12</v>
+      </c>
+      <c r="AX61">
+        <v>12</v>
+      </c>
+      <c r="AY61">
+        <v>12</v>
+      </c>
+      <c r="AZ61">
+        <v>12</v>
+      </c>
+      <c r="BA61">
+        <v>12</v>
+      </c>
+      <c r="BB61">
+        <v>12</v>
+      </c>
+      <c r="BC61">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="62" ht="19.5">
-      <c s="6" r="G62"/>
+      <c t="s" r="A62">
+        <v>6</v>
+      </c>
+      <c t="s" r="C62">
+        <v>19</v>
+      </c>
+      <c t="s" r="D62">
+        <v>41</v>
+      </c>
+      <c t="s" r="E62">
+        <v>40</v>
+      </c>
+      <c t="s" r="F62">
+        <v>10</v>
+      </c>
+      <c s="5" r="G62"/>
+      <c r="U62">
+        <v>12</v>
+      </c>
+      <c r="V62">
+        <v>12</v>
+      </c>
+      <c r="W62">
+        <v>12</v>
+      </c>
+      <c r="X62">
+        <v>12</v>
+      </c>
+      <c r="Y62">
+        <v>12</v>
+      </c>
+      <c r="Z62">
+        <v>12</v>
+      </c>
+      <c r="AA62">
+        <v>12</v>
+      </c>
+      <c r="AB62">
+        <v>12</v>
+      </c>
+      <c r="AC62">
+        <v>12</v>
+      </c>
+      <c r="AD62">
+        <v>12</v>
+      </c>
+      <c r="AE62">
+        <v>12</v>
+      </c>
+      <c r="AF62">
+        <v>12</v>
+      </c>
+      <c r="AG62">
+        <v>12</v>
+      </c>
+      <c r="AQ62">
+        <v>12</v>
+      </c>
+      <c r="AR62">
+        <v>12</v>
+      </c>
+      <c r="AS62">
+        <v>12</v>
+      </c>
+      <c r="AT62">
+        <v>12</v>
+      </c>
+      <c r="AU62">
+        <v>12</v>
+      </c>
+      <c r="AV62">
+        <v>12</v>
+      </c>
+      <c r="AW62">
+        <v>12</v>
+      </c>
+      <c r="AX62">
+        <v>12</v>
+      </c>
+      <c r="AY62">
+        <v>12</v>
+      </c>
+      <c r="AZ62">
+        <v>12</v>
+      </c>
+      <c r="BA62">
+        <v>12</v>
+      </c>
+      <c r="BB62">
+        <v>12</v>
+      </c>
+      <c r="BC62">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="63" ht="19.5">
-      <c s="6" r="G63"/>
+      <c t="s" r="A63">
+        <v>6</v>
+      </c>
+      <c t="s" r="C63">
+        <v>20</v>
+      </c>
+      <c t="s" r="D63">
+        <v>41</v>
+      </c>
+      <c t="s" r="E63">
+        <v>40</v>
+      </c>
+      <c t="s" r="F63">
+        <v>10</v>
+      </c>
+      <c s="5" r="G63"/>
+      <c r="U63">
+        <v>12</v>
+      </c>
+      <c r="V63">
+        <v>12</v>
+      </c>
+      <c r="W63">
+        <v>12</v>
+      </c>
+      <c r="X63">
+        <v>12</v>
+      </c>
+      <c r="Y63">
+        <v>12</v>
+      </c>
+      <c r="Z63">
+        <v>12</v>
+      </c>
+      <c r="AA63">
+        <v>12</v>
+      </c>
+      <c r="AB63">
+        <v>12</v>
+      </c>
+      <c r="AC63">
+        <v>12</v>
+      </c>
+      <c r="AD63">
+        <v>12</v>
+      </c>
+      <c r="AE63">
+        <v>12</v>
+      </c>
+      <c r="AF63">
+        <v>12</v>
+      </c>
+      <c r="AG63">
+        <v>12</v>
+      </c>
+      <c r="AQ63">
+        <v>12</v>
+      </c>
+      <c r="AR63">
+        <v>12</v>
+      </c>
+      <c r="AS63">
+        <v>12</v>
+      </c>
+      <c r="AT63">
+        <v>12</v>
+      </c>
+      <c r="AU63">
+        <v>12</v>
+      </c>
+      <c r="AV63">
+        <v>12</v>
+      </c>
+      <c r="AW63">
+        <v>12</v>
+      </c>
+      <c r="AX63">
+        <v>12</v>
+      </c>
+      <c r="AY63">
+        <v>12</v>
+      </c>
+      <c r="AZ63">
+        <v>12</v>
+      </c>
+      <c r="BA63">
+        <v>12</v>
+      </c>
+      <c r="BB63">
+        <v>12</v>
+      </c>
+      <c r="BC63">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" r="64" ht="19.5">
-      <c s="6" r="G64"/>
+      <c s="5" r="G64"/>
     </row>
     <row customHeight="1" r="65" ht="19.5">
-      <c s="6" r="G65"/>
+      <c s="5" r="G65"/>
     </row>
     <row customHeight="1" r="66" ht="19.5">
-      <c s="6" r="G66"/>
+      <c s="5" r="G66"/>
     </row>
     <row customHeight="1" r="67" ht="19.5">
-      <c s="6" r="G67"/>
+      <c s="5" r="G67"/>
     </row>
     <row customHeight="1" r="68" ht="19.5">
-      <c s="6" r="G68"/>
+      <c s="5" r="G68"/>
     </row>
     <row customHeight="1" r="69" ht="19.5">
-      <c s="6" r="G69"/>
+      <c s="5" r="G69"/>
     </row>
     <row customHeight="1" r="70" ht="19.5">
-      <c s="6" r="G70"/>
+      <c s="5" r="G70"/>
     </row>
     <row customHeight="1" r="71" ht="19.5">
-      <c s="6" r="G71"/>
+      <c s="5" r="G71"/>
     </row>
     <row customHeight="1" r="72" ht="19.5">
-      <c s="6" r="G72"/>
+      <c s="5" r="G72"/>
     </row>
     <row customHeight="1" r="73" ht="19.5">
-      <c s="6" r="G73"/>
+      <c s="5" r="G73"/>
     </row>
     <row customHeight="1" r="74" ht="19.5">
-      <c s="6" r="G74"/>
+      <c s="5" r="G74"/>
     </row>
     <row customHeight="1" r="75" ht="19.5">
-      <c s="6" r="G75"/>
+      <c s="5" r="G75"/>
     </row>
     <row customHeight="1" r="76" ht="19.5">
-      <c s="6" r="G76"/>
+      <c s="5" r="G76"/>
     </row>
     <row customHeight="1" r="77" ht="19.5">
-      <c s="6" r="G77"/>
+      <c s="5" r="G77"/>
     </row>
     <row customHeight="1" r="78" ht="19.5">
-      <c s="6" r="G78"/>
+      <c s="5" r="G78"/>
     </row>
     <row customHeight="1" r="79" ht="19.5">
-      <c s="6" r="G79"/>
+      <c s="5" r="G79"/>
     </row>
     <row customHeight="1" r="80" ht="19.5">
-      <c s="6" r="G80"/>
+      <c s="5" r="G80"/>
     </row>
     <row customHeight="1" r="81" ht="19.5">
-      <c s="6" r="G81"/>
+      <c s="5" r="G81"/>
     </row>
     <row customHeight="1" r="82" ht="19.5">
-      <c s="6" r="G82"/>
+      <c s="5" r="G82"/>
     </row>
     <row customHeight="1" r="83" ht="19.5">
-      <c s="6" r="G83"/>
+      <c s="5" r="G83"/>
     </row>
     <row customHeight="1" r="84" ht="19.5">
-      <c s="6" r="G84"/>
+      <c s="5" r="G84"/>
     </row>
     <row customHeight="1" r="85" ht="19.5">
-      <c s="6" r="G85"/>
+      <c s="5" r="G85"/>
     </row>
     <row customHeight="1" r="86" ht="19.5">
-      <c s="6" r="G86"/>
+      <c s="5" r="G86"/>
     </row>
     <row customHeight="1" r="87" ht="19.5">
-      <c s="6" r="G87"/>
+      <c s="5" r="G87"/>
     </row>
     <row customHeight="1" r="88" ht="19.5">
-      <c s="6" r="G88"/>
+      <c s="5" r="G88"/>
     </row>
     <row customHeight="1" r="89" ht="19.5">
-      <c s="6" r="G89"/>
+      <c s="5" r="G89"/>
     </row>
     <row customHeight="1" r="90" ht="19.5">
-      <c s="6" r="G90"/>
+      <c s="5" r="G90"/>
     </row>
     <row customHeight="1" r="91" ht="19.5">
-      <c s="6" r="G91"/>
+      <c s="5" r="G91"/>
     </row>
     <row customHeight="1" r="92" ht="19.5">
-      <c s="6" r="G92"/>
+      <c s="5" r="G92"/>
     </row>
     <row customHeight="1" r="93" ht="19.5">
-      <c s="6" r="G93"/>
+      <c s="5" r="G93"/>
     </row>
     <row customHeight="1" r="94" ht="19.5">
-      <c s="6" r="G94"/>
+      <c s="5" r="G94"/>
     </row>
     <row customHeight="1" r="95" ht="19.5">
-      <c s="6" r="G95"/>
+      <c s="5" r="G95"/>
     </row>
     <row customHeight="1" r="96" ht="19.5">
-      <c s="6" r="G96"/>
+      <c s="5" r="G96"/>
     </row>
     <row customHeight="1" r="97" ht="19.5">
-      <c s="6" r="G97"/>
+      <c s="5" r="G97"/>
     </row>
     <row customHeight="1" r="98" ht="19.5">
-      <c s="6" r="G98"/>
+      <c s="5" r="G98"/>
     </row>
     <row customHeight="1" r="99" ht="19.5">
-      <c s="6" r="G99"/>
+      <c s="5" r="G99"/>
     </row>
     <row customHeight="1" r="100" ht="19.5">
-      <c s="6" r="G100"/>
+      <c s="5" r="G100"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2 D2 E2 F2 H2 I2 J2 K2 L2 M2 N2 O2 P2 Q2 R2 S2 T2 U2 V2 W2 X2 Y2 Z2 AA2 AB2 AC2 AD2 AE2 AF2 AG2 AH2 AI2 AJ2 AK2 AL2 AM2 AN2 AO2 AP2 AQ2 AR2 AS2 AT2 AU2 AV2 AW2 AX2 AY2 AZ2 BA2 BB2 BC2 BD2 BE2 BF2 BG2 BH2">
-    <cfRule timePeriod="last7Days" priority="1" type="timePeriod" stopIfTrue="1" dxfId="0"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33 A34 A35 A36 A37 A38 A39 A40 A41 A42 A43 A44 A45 A46 A47 A48 A49 A50 A51 A52 A53 A54 A55 A56 A57 A58 A59 A60 A61 A62 A63 A64 A65 A66 A67 A68 A69 A70 A71 A72 A73 A74 A75 A76 A77 A78 A79 A80 A81 A82 A83 A84 A85 A86 A87 A88 A89 A90 A91 A92 A93 A94 A95 A96 A97 A98 A99 A100">
-    <cfRule text="Booked" priority="1" type="containsText" operator="containsText" stopIfTrue="1" dxfId="3">
+    <cfRule text="Booked" priority="1" type="containsText" operator="containsText" stopIfTrue="1" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("Booked", A1)))</formula>
     </cfRule>
-    <cfRule text="Pipeline" priority="2" type="containsText" operator="containsText" stopIfTrue="1" dxfId="4">
+    <cfRule text="Pipeline" priority="2" type="containsText" operator="containsText" stopIfTrue="1" dxfId="1">
       <formula>NOT(ISERROR(SEARCH("Pipeline", A1)))</formula>
     </cfRule>
+    <cfRule text="Recurring" priority="3" type="containsText" operator="containsText" stopIfTrue="1" dxfId="2">
+      <formula>NOT(ISERROR(SEARCH("Recurring", A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2 D2 E2 F2 H2 I2 J2 K2 L2 M2 N2 O2 P2 Q2 R2 S2 T2 U2 V2 W2 X2 Y2 Z2 AA2 AB2 AC2 AD2 AE2 AF2 AG2 AH2 AI2 AJ2 AK2 AL2 AM2 AN2 AO2 AP2 AQ2 AR2 AS2 AT2 AU2 AV2 AW2 AX2 AY2 AZ2 BA2 BB2 BC2 BD2 BE2 BF2 BG2 BH2">
+    <cfRule timePeriod="last7Days" priority="1" type="timePeriod" stopIfTrue="1" dxfId="3"/>
   </conditionalFormatting>
 </worksheet>
 </file>
</xml_diff>